<commit_message>
Update of the metadata schema file
</commit_message>
<xml_diff>
--- a/Metadata_Schema_for_openBIS.xlsx
+++ b/Metadata_Schema_for_openBIS.xlsx
@@ -9,17 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22050" windowHeight="8355" tabRatio="699"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22050" windowHeight="8355" tabRatio="699" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata Schema" sheetId="7" r:id="rId1"/>
     <sheet name="Metadata Updates" sheetId="15" r:id="rId2"/>
     <sheet name="Ontology - definition" sheetId="8" r:id="rId3"/>
-    <sheet name="Ontology - schema.org" sheetId="16" r:id="rId4"/>
-    <sheet name="openBIS - parameters" sheetId="10" r:id="rId5"/>
-    <sheet name="openBIS - vocabulary" sheetId="11" r:id="rId6"/>
-    <sheet name="openBIS - vocabulary terms" sheetId="13" r:id="rId7"/>
-    <sheet name="Legend" sheetId="14" r:id="rId8"/>
+    <sheet name="openBIS - parameters" sheetId="10" r:id="rId4"/>
+    <sheet name="openBIS - vocabulary" sheetId="11" r:id="rId5"/>
+    <sheet name="openBIS - vocabulary terms" sheetId="13" r:id="rId6"/>
+    <sheet name="Legend" sheetId="14" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6252" uniqueCount="1983">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6131" uniqueCount="1970">
   <si>
     <t>duration</t>
   </si>
@@ -5923,45 +5922,6 @@
   </si>
   <si>
     <t>hasPart-WaferSubstrate</t>
-  </si>
-  <si>
-    <t>https://schema.org/MonetaryGrant</t>
-  </si>
-  <si>
-    <t>https://schema.org/Article</t>
-  </si>
-  <si>
-    <t>https://schema.org/author</t>
-  </si>
-  <si>
-    <t>https://schema.org/Organization</t>
-  </si>
-  <si>
-    <t>https://schema.org/ResearchOrganization</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> or Group?</t>
-  </si>
-  <si>
-    <t>https://schema.org/MolecularEntity</t>
-  </si>
-  <si>
-    <t>https://schema.org/instrument</t>
-  </si>
-  <si>
-    <t>https://schema.org/SoftwareSourceCode</t>
-  </si>
-  <si>
-    <t>https://schema.org/MoveAction</t>
-  </si>
-  <si>
-    <t>error</t>
-  </si>
-  <si>
-    <t>https://schema.org/error</t>
-  </si>
-  <si>
-    <t>https://schema.org/Manuscript</t>
   </si>
   <si>
     <t>Connection to Crystal object</t>
@@ -6039,7 +5999,7 @@
       <name val="Segoe UI"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -6068,12 +6028,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor theme="9"/>
       </patternFill>
     </fill>
     <fill>
@@ -6206,7 +6160,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -6380,19 +6334,14 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -7121,7 +7070,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:K649"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A572" zoomScale="121" zoomScaleNormal="98" workbookViewId="0">
+    <sheetView topLeftCell="A572" zoomScale="121" zoomScaleNormal="98" workbookViewId="0">
       <selection activeCell="D591" sqref="D591"/>
     </sheetView>
   </sheetViews>
@@ -11023,7 +10972,7 @@
         <v>100</v>
       </c>
       <c r="D120" s="4" t="s">
-        <v>1977</v>
+        <v>1964</v>
       </c>
       <c r="E120" s="34" t="s">
         <v>1065</v>
@@ -15636,7 +15585,7 @@
         <v>100</v>
       </c>
       <c r="D253" s="4" t="s">
-        <v>1978</v>
+        <v>1965</v>
       </c>
       <c r="E253" s="4" t="s">
         <v>1066</v>
@@ -26609,73 +26558,73 @@
       </c>
     </row>
     <row r="566" spans="1:11" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A566" s="93" t="s">
+      <c r="A566" s="88" t="s">
         <v>225</v>
       </c>
-      <c r="B566" s="90" t="s">
+      <c r="B566" s="85" t="s">
         <v>990</v>
       </c>
-      <c r="C566" s="90" t="s">
+      <c r="C566" s="85" t="s">
         <v>101</v>
       </c>
-      <c r="D566" s="90" t="s">
+      <c r="D566" s="85" t="s">
         <v>406</v>
       </c>
-      <c r="E566" s="90" t="s">
+      <c r="E566" s="85" t="s">
         <v>893</v>
       </c>
-      <c r="F566" s="90" t="s">
+      <c r="F566" s="85" t="s">
         <v>896</v>
       </c>
-      <c r="G566" s="93" t="s">
+      <c r="G566" s="88" t="s">
         <v>960</v>
       </c>
-      <c r="H566" s="90"/>
-      <c r="I566" s="90" t="str">
-        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[openBIS]], 'openBIS - parameters'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
-        <v>Exists</v>
-      </c>
-      <c r="J566" s="91" t="str">
-        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[Ontology]], 'Ontology - definition'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
-        <v>Exists</v>
-      </c>
-      <c r="K566" s="92" t="str">
+      <c r="H566" s="85"/>
+      <c r="I566" s="85" t="str">
+        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[openBIS]], 'openBIS - parameters'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
+        <v>Exists</v>
+      </c>
+      <c r="J566" s="86" t="str">
+        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[Ontology]], 'Ontology - definition'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
+        <v>Exists</v>
+      </c>
+      <c r="K566" s="87" t="str">
         <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISBLANK(VLOOKUP(Table1[[#This Row],[Ontology]],'Ontology - definition'!A:B,2,FALSE)),"Doesn't Exist","Exists"),"")</f>
         <v>Exists</v>
       </c>
     </row>
     <row r="567" spans="1:11" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A567" s="93" t="s">
+      <c r="A567" s="88" t="s">
         <v>434</v>
       </c>
-      <c r="B567" s="90" t="s">
+      <c r="B567" s="85" t="s">
         <v>990</v>
       </c>
-      <c r="C567" s="90" t="s">
+      <c r="C567" s="85" t="s">
         <v>101</v>
       </c>
-      <c r="D567" s="90" t="s">
+      <c r="D567" s="85" t="s">
         <v>224</v>
       </c>
-      <c r="E567" s="90" t="s">
+      <c r="E567" s="85" t="s">
         <v>903</v>
       </c>
-      <c r="F567" s="90" t="s">
+      <c r="F567" s="85" t="s">
         <v>904</v>
       </c>
-      <c r="G567" s="93" t="s">
+      <c r="G567" s="88" t="s">
         <v>966</v>
       </c>
-      <c r="H567" s="90"/>
-      <c r="I567" s="90" t="str">
-        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[openBIS]], 'openBIS - parameters'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
-        <v>Exists</v>
-      </c>
-      <c r="J567" s="91" t="str">
-        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[Ontology]], 'Ontology - definition'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
-        <v>Exists</v>
-      </c>
-      <c r="K567" s="92" t="str">
+      <c r="H567" s="85"/>
+      <c r="I567" s="85" t="str">
+        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[openBIS]], 'openBIS - parameters'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
+        <v>Exists</v>
+      </c>
+      <c r="J567" s="86" t="str">
+        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[Ontology]], 'Ontology - definition'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
+        <v>Exists</v>
+      </c>
+      <c r="K567" s="87" t="str">
         <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISBLANK(VLOOKUP(Table1[[#This Row],[Ontology]],'Ontology - definition'!A:B,2,FALSE)),"Doesn't Exist","Exists"),"")</f>
         <v>Exists</v>
       </c>
@@ -27321,73 +27270,73 @@
       </c>
     </row>
     <row r="586" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A586" s="93" t="s">
+      <c r="A586" s="88" t="s">
         <v>225</v>
       </c>
-      <c r="B586" s="90" t="s">
+      <c r="B586" s="85" t="s">
         <v>990</v>
       </c>
-      <c r="C586" s="90" t="s">
+      <c r="C586" s="85" t="s">
         <v>101</v>
       </c>
-      <c r="D586" s="90" t="s">
+      <c r="D586" s="85" t="s">
         <v>406</v>
       </c>
-      <c r="E586" s="90" t="s">
+      <c r="E586" s="85" t="s">
         <v>893</v>
       </c>
-      <c r="F586" s="90" t="s">
+      <c r="F586" s="85" t="s">
         <v>896</v>
       </c>
-      <c r="G586" s="93" t="s">
+      <c r="G586" s="88" t="s">
         <v>960</v>
       </c>
-      <c r="H586" s="90"/>
-      <c r="I586" s="90" t="str">
-        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[openBIS]], 'openBIS - parameters'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
-        <v>Exists</v>
-      </c>
-      <c r="J586" s="91" t="str">
-        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[Ontology]], 'Ontology - definition'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
-        <v>Exists</v>
-      </c>
-      <c r="K586" s="92" t="str">
+      <c r="H586" s="85"/>
+      <c r="I586" s="85" t="str">
+        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[openBIS]], 'openBIS - parameters'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
+        <v>Exists</v>
+      </c>
+      <c r="J586" s="86" t="str">
+        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[Ontology]], 'Ontology - definition'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
+        <v>Exists</v>
+      </c>
+      <c r="K586" s="87" t="str">
         <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISBLANK(VLOOKUP(Table1[[#This Row],[Ontology]],'Ontology - definition'!A:B,2,FALSE)),"Doesn't Exist","Exists"),"")</f>
         <v>Exists</v>
       </c>
     </row>
     <row r="587" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A587" s="93" t="s">
+      <c r="A587" s="88" t="s">
         <v>434</v>
       </c>
-      <c r="B587" s="90" t="s">
+      <c r="B587" s="85" t="s">
         <v>990</v>
       </c>
-      <c r="C587" s="90" t="s">
+      <c r="C587" s="85" t="s">
         <v>101</v>
       </c>
-      <c r="D587" s="90" t="s">
+      <c r="D587" s="85" t="s">
         <v>224</v>
       </c>
-      <c r="E587" s="90" t="s">
+      <c r="E587" s="85" t="s">
         <v>903</v>
       </c>
-      <c r="F587" s="90" t="s">
+      <c r="F587" s="85" t="s">
         <v>904</v>
       </c>
-      <c r="G587" s="93" t="s">
+      <c r="G587" s="88" t="s">
         <v>966</v>
       </c>
-      <c r="H587" s="90"/>
-      <c r="I587" s="90" t="str">
-        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[openBIS]], 'openBIS - parameters'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
-        <v>Exists</v>
-      </c>
-      <c r="J587" s="91" t="str">
-        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[Ontology]], 'Ontology - definition'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
-        <v>Exists</v>
-      </c>
-      <c r="K587" s="92" t="str">
+      <c r="H587" s="85"/>
+      <c r="I587" s="85" t="str">
+        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[openBIS]], 'openBIS - parameters'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
+        <v>Exists</v>
+      </c>
+      <c r="J587" s="86" t="str">
+        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[Ontology]], 'Ontology - definition'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
+        <v>Exists</v>
+      </c>
+      <c r="K587" s="87" t="str">
         <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISBLANK(VLOOKUP(Table1[[#This Row],[Ontology]],'Ontology - definition'!A:B,2,FALSE)),"Doesn't Exist","Exists"),"")</f>
         <v>Exists</v>
       </c>
@@ -27768,80 +27717,80 @@
       </c>
     </row>
     <row r="599" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A599" s="93" t="s">
+      <c r="A599" s="88" t="s">
         <v>225</v>
       </c>
-      <c r="B599" s="90" t="s">
+      <c r="B599" s="85" t="s">
         <v>990</v>
       </c>
-      <c r="C599" s="90" t="s">
+      <c r="C599" s="85" t="s">
         <v>101</v>
       </c>
-      <c r="D599" s="90" t="s">
+      <c r="D599" s="85" t="s">
         <v>406</v>
       </c>
-      <c r="E599" s="90" t="s">
+      <c r="E599" s="85" t="s">
         <v>893</v>
       </c>
-      <c r="F599" s="90" t="s">
+      <c r="F599" s="85" t="s">
         <v>896</v>
       </c>
-      <c r="G599" s="93" t="s">
+      <c r="G599" s="88" t="s">
         <v>960</v>
       </c>
-      <c r="H599" s="90"/>
-      <c r="I599" s="90" t="str">
-        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[openBIS]], 'openBIS - parameters'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
-        <v>Exists</v>
-      </c>
-      <c r="J599" s="91" t="str">
-        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[Ontology]], 'Ontology - definition'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
-        <v>Exists</v>
-      </c>
-      <c r="K599" s="92" t="str">
+      <c r="H599" s="85"/>
+      <c r="I599" s="85" t="str">
+        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[openBIS]], 'openBIS - parameters'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
+        <v>Exists</v>
+      </c>
+      <c r="J599" s="86" t="str">
+        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[Ontology]], 'Ontology - definition'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
+        <v>Exists</v>
+      </c>
+      <c r="K599" s="87" t="str">
         <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISBLANK(VLOOKUP(Table1[[#This Row],[Ontology]],'Ontology - definition'!A:B,2,FALSE)),"Doesn't Exist","Exists"),"")</f>
         <v>Exists</v>
       </c>
     </row>
     <row r="600" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A600" s="93" t="s">
+      <c r="A600" s="88" t="s">
         <v>434</v>
       </c>
-      <c r="B600" s="90" t="s">
+      <c r="B600" s="85" t="s">
         <v>990</v>
       </c>
-      <c r="C600" s="90" t="s">
+      <c r="C600" s="85" t="s">
         <v>101</v>
       </c>
-      <c r="D600" s="90" t="s">
+      <c r="D600" s="85" t="s">
         <v>224</v>
       </c>
-      <c r="E600" s="90" t="s">
+      <c r="E600" s="85" t="s">
         <v>903</v>
       </c>
-      <c r="F600" s="90" t="s">
+      <c r="F600" s="85" t="s">
         <v>904</v>
       </c>
-      <c r="G600" s="93" t="s">
+      <c r="G600" s="88" t="s">
         <v>966</v>
       </c>
-      <c r="H600" s="90"/>
-      <c r="I600" s="90" t="str">
-        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[openBIS]], 'openBIS - parameters'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
-        <v>Exists</v>
-      </c>
-      <c r="J600" s="91" t="str">
-        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[Ontology]], 'Ontology - definition'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
-        <v>Exists</v>
-      </c>
-      <c r="K600" s="92" t="str">
+      <c r="H600" s="85"/>
+      <c r="I600" s="85" t="str">
+        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[openBIS]], 'openBIS - parameters'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
+        <v>Exists</v>
+      </c>
+      <c r="J600" s="86" t="str">
+        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[Ontology]], 'Ontology - definition'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
+        <v>Exists</v>
+      </c>
+      <c r="K600" s="87" t="str">
         <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISBLANK(VLOOKUP(Table1[[#This Row],[Ontology]],'Ontology - definition'!A:B,2,FALSE)),"Doesn't Exist","Exists"),"")</f>
         <v>Exists</v>
       </c>
     </row>
     <row r="601" spans="1:11" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A601" s="4" t="s">
-        <v>1979</v>
+        <v>1966</v>
       </c>
       <c r="B601" s="4" t="s">
         <v>1575</v>
@@ -28179,73 +28128,73 @@
       </c>
     </row>
     <row r="611" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A611" s="93" t="s">
+      <c r="A611" s="88" t="s">
         <v>225</v>
       </c>
-      <c r="B611" s="90" t="s">
+      <c r="B611" s="85" t="s">
         <v>990</v>
       </c>
-      <c r="C611" s="90" t="s">
+      <c r="C611" s="85" t="s">
         <v>101</v>
       </c>
-      <c r="D611" s="90" t="s">
+      <c r="D611" s="85" t="s">
         <v>406</v>
       </c>
-      <c r="E611" s="90" t="s">
+      <c r="E611" s="85" t="s">
         <v>893</v>
       </c>
-      <c r="F611" s="90" t="s">
+      <c r="F611" s="85" t="s">
         <v>896</v>
       </c>
-      <c r="G611" s="93" t="s">
+      <c r="G611" s="88" t="s">
         <v>960</v>
       </c>
-      <c r="H611" s="90"/>
-      <c r="I611" s="90" t="str">
-        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[openBIS]], 'openBIS - parameters'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
-        <v>Exists</v>
-      </c>
-      <c r="J611" s="91" t="str">
-        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[Ontology]], 'Ontology - definition'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
-        <v>Exists</v>
-      </c>
-      <c r="K611" s="92" t="str">
+      <c r="H611" s="85"/>
+      <c r="I611" s="85" t="str">
+        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[openBIS]], 'openBIS - parameters'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
+        <v>Exists</v>
+      </c>
+      <c r="J611" s="86" t="str">
+        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[Ontology]], 'Ontology - definition'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
+        <v>Exists</v>
+      </c>
+      <c r="K611" s="87" t="str">
         <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISBLANK(VLOOKUP(Table1[[#This Row],[Ontology]],'Ontology - definition'!A:B,2,FALSE)),"Doesn't Exist","Exists"),"")</f>
         <v>Exists</v>
       </c>
     </row>
     <row r="612" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A612" s="93" t="s">
+      <c r="A612" s="88" t="s">
         <v>434</v>
       </c>
-      <c r="B612" s="90" t="s">
+      <c r="B612" s="85" t="s">
         <v>990</v>
       </c>
-      <c r="C612" s="90" t="s">
+      <c r="C612" s="85" t="s">
         <v>101</v>
       </c>
-      <c r="D612" s="90" t="s">
+      <c r="D612" s="85" t="s">
         <v>224</v>
       </c>
-      <c r="E612" s="90" t="s">
+      <c r="E612" s="85" t="s">
         <v>903</v>
       </c>
-      <c r="F612" s="90" t="s">
+      <c r="F612" s="85" t="s">
         <v>904</v>
       </c>
-      <c r="G612" s="93" t="s">
+      <c r="G612" s="88" t="s">
         <v>966</v>
       </c>
-      <c r="H612" s="90"/>
-      <c r="I612" s="90" t="str">
-        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[openBIS]], 'openBIS - parameters'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
-        <v>Exists</v>
-      </c>
-      <c r="J612" s="91" t="str">
-        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[Ontology]], 'Ontology - definition'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
-        <v>Exists</v>
-      </c>
-      <c r="K612" s="92" t="str">
+      <c r="H612" s="85"/>
+      <c r="I612" s="85" t="str">
+        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[openBIS]], 'openBIS - parameters'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
+        <v>Exists</v>
+      </c>
+      <c r="J612" s="86" t="str">
+        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[Ontology]], 'Ontology - definition'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
+        <v>Exists</v>
+      </c>
+      <c r="K612" s="87" t="str">
         <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISBLANK(VLOOKUP(Table1[[#This Row],[Ontology]],'Ontology - definition'!A:B,2,FALSE)),"Doesn't Exist","Exists"),"")</f>
         <v>Exists</v>
       </c>
@@ -28550,73 +28499,73 @@
       </c>
     </row>
     <row r="622" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A622" s="93" t="s">
+      <c r="A622" s="88" t="s">
         <v>225</v>
       </c>
-      <c r="B622" s="90" t="s">
+      <c r="B622" s="85" t="s">
         <v>990</v>
       </c>
-      <c r="C622" s="90" t="s">
+      <c r="C622" s="85" t="s">
         <v>101</v>
       </c>
-      <c r="D622" s="90" t="s">
+      <c r="D622" s="85" t="s">
         <v>406</v>
       </c>
-      <c r="E622" s="90" t="s">
+      <c r="E622" s="85" t="s">
         <v>893</v>
       </c>
-      <c r="F622" s="90" t="s">
+      <c r="F622" s="85" t="s">
         <v>896</v>
       </c>
-      <c r="G622" s="93" t="s">
+      <c r="G622" s="88" t="s">
         <v>960</v>
       </c>
-      <c r="H622" s="90"/>
-      <c r="I622" s="90" t="str">
-        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[openBIS]], 'openBIS - parameters'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
-        <v>Exists</v>
-      </c>
-      <c r="J622" s="91" t="str">
-        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[Ontology]], 'Ontology - definition'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
-        <v>Exists</v>
-      </c>
-      <c r="K622" s="92" t="str">
+      <c r="H622" s="85"/>
+      <c r="I622" s="85" t="str">
+        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[openBIS]], 'openBIS - parameters'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
+        <v>Exists</v>
+      </c>
+      <c r="J622" s="86" t="str">
+        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[Ontology]], 'Ontology - definition'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
+        <v>Exists</v>
+      </c>
+      <c r="K622" s="87" t="str">
         <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISBLANK(VLOOKUP(Table1[[#This Row],[Ontology]],'Ontology - definition'!A:B,2,FALSE)),"Doesn't Exist","Exists"),"")</f>
         <v>Exists</v>
       </c>
     </row>
     <row r="623" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A623" s="93" t="s">
+      <c r="A623" s="88" t="s">
         <v>434</v>
       </c>
-      <c r="B623" s="90" t="s">
+      <c r="B623" s="85" t="s">
         <v>990</v>
       </c>
-      <c r="C623" s="90" t="s">
+      <c r="C623" s="85" t="s">
         <v>101</v>
       </c>
-      <c r="D623" s="90" t="s">
+      <c r="D623" s="85" t="s">
         <v>224</v>
       </c>
-      <c r="E623" s="90" t="s">
+      <c r="E623" s="85" t="s">
         <v>903</v>
       </c>
-      <c r="F623" s="90" t="s">
+      <c r="F623" s="85" t="s">
         <v>904</v>
       </c>
-      <c r="G623" s="93" t="s">
+      <c r="G623" s="88" t="s">
         <v>966</v>
       </c>
-      <c r="H623" s="90"/>
-      <c r="I623" s="90" t="str">
-        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[openBIS]], 'openBIS - parameters'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
-        <v>Exists</v>
-      </c>
-      <c r="J623" s="91" t="str">
-        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[Ontology]], 'Ontology - definition'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
-        <v>Exists</v>
-      </c>
-      <c r="K623" s="92" t="str">
+      <c r="H623" s="85"/>
+      <c r="I623" s="85" t="str">
+        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[openBIS]], 'openBIS - parameters'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
+        <v>Exists</v>
+      </c>
+      <c r="J623" s="86" t="str">
+        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[Ontology]], 'Ontology - definition'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
+        <v>Exists</v>
+      </c>
+      <c r="K623" s="87" t="str">
         <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISBLANK(VLOOKUP(Table1[[#This Row],[Ontology]],'Ontology - definition'!A:B,2,FALSE)),"Doesn't Exist","Exists"),"")</f>
         <v>Exists</v>
       </c>
@@ -28959,73 +28908,73 @@
       </c>
     </row>
     <row r="634" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A634" s="93" t="s">
+      <c r="A634" s="88" t="s">
         <v>225</v>
       </c>
-      <c r="B634" s="90" t="s">
+      <c r="B634" s="85" t="s">
         <v>990</v>
       </c>
-      <c r="C634" s="90" t="s">
+      <c r="C634" s="85" t="s">
         <v>101</v>
       </c>
-      <c r="D634" s="90" t="s">
+      <c r="D634" s="85" t="s">
         <v>406</v>
       </c>
-      <c r="E634" s="90" t="s">
+      <c r="E634" s="85" t="s">
         <v>893</v>
       </c>
-      <c r="F634" s="90" t="s">
+      <c r="F634" s="85" t="s">
         <v>896</v>
       </c>
-      <c r="G634" s="93" t="s">
+      <c r="G634" s="88" t="s">
         <v>960</v>
       </c>
-      <c r="H634" s="90"/>
-      <c r="I634" s="90" t="str">
-        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[openBIS]], 'openBIS - parameters'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
-        <v>Exists</v>
-      </c>
-      <c r="J634" s="91" t="str">
-        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[Ontology]], 'Ontology - definition'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
-        <v>Exists</v>
-      </c>
-      <c r="K634" s="92" t="str">
+      <c r="H634" s="85"/>
+      <c r="I634" s="85" t="str">
+        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[openBIS]], 'openBIS - parameters'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
+        <v>Exists</v>
+      </c>
+      <c r="J634" s="86" t="str">
+        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[Ontology]], 'Ontology - definition'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
+        <v>Exists</v>
+      </c>
+      <c r="K634" s="87" t="str">
         <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISBLANK(VLOOKUP(Table1[[#This Row],[Ontology]],'Ontology - definition'!A:B,2,FALSE)),"Doesn't Exist","Exists"),"")</f>
         <v>Exists</v>
       </c>
     </row>
     <row r="635" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A635" s="93" t="s">
+      <c r="A635" s="88" t="s">
         <v>434</v>
       </c>
-      <c r="B635" s="90" t="s">
+      <c r="B635" s="85" t="s">
         <v>990</v>
       </c>
-      <c r="C635" s="90" t="s">
+      <c r="C635" s="85" t="s">
         <v>101</v>
       </c>
-      <c r="D635" s="90" t="s">
+      <c r="D635" s="85" t="s">
         <v>224</v>
       </c>
-      <c r="E635" s="90" t="s">
+      <c r="E635" s="85" t="s">
         <v>903</v>
       </c>
-      <c r="F635" s="90" t="s">
+      <c r="F635" s="85" t="s">
         <v>904</v>
       </c>
-      <c r="G635" s="93" t="s">
+      <c r="G635" s="88" t="s">
         <v>966</v>
       </c>
-      <c r="H635" s="90"/>
-      <c r="I635" s="90" t="str">
-        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[openBIS]], 'openBIS - parameters'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
-        <v>Exists</v>
-      </c>
-      <c r="J635" s="91" t="str">
-        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[Ontology]], 'Ontology - definition'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
-        <v>Exists</v>
-      </c>
-      <c r="K635" s="92" t="str">
+      <c r="H635" s="85"/>
+      <c r="I635" s="85" t="str">
+        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[openBIS]], 'openBIS - parameters'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
+        <v>Exists</v>
+      </c>
+      <c r="J635" s="86" t="str">
+        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[Ontology]], 'Ontology - definition'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
+        <v>Exists</v>
+      </c>
+      <c r="K635" s="87" t="str">
         <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISBLANK(VLOOKUP(Table1[[#This Row],[Ontology]],'Ontology - definition'!A:B,2,FALSE)),"Doesn't Exist","Exists"),"")</f>
         <v>Exists</v>
       </c>
@@ -29121,73 +29070,73 @@
       </c>
     </row>
     <row r="639" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A639" s="93" t="s">
+      <c r="A639" s="88" t="s">
         <v>225</v>
       </c>
-      <c r="B639" s="90" t="s">
+      <c r="B639" s="85" t="s">
         <v>990</v>
       </c>
-      <c r="C639" s="90" t="s">
+      <c r="C639" s="85" t="s">
         <v>101</v>
       </c>
-      <c r="D639" s="90" t="s">
+      <c r="D639" s="85" t="s">
         <v>406</v>
       </c>
-      <c r="E639" s="90" t="s">
+      <c r="E639" s="85" t="s">
         <v>893</v>
       </c>
-      <c r="F639" s="90" t="s">
+      <c r="F639" s="85" t="s">
         <v>896</v>
       </c>
-      <c r="G639" s="93" t="s">
+      <c r="G639" s="88" t="s">
         <v>960</v>
       </c>
-      <c r="H639" s="90"/>
-      <c r="I639" s="90" t="str">
-        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[openBIS]], 'openBIS - parameters'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
-        <v>Exists</v>
-      </c>
-      <c r="J639" s="91" t="str">
-        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[Ontology]], 'Ontology - definition'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
-        <v>Exists</v>
-      </c>
-      <c r="K639" s="92" t="str">
+      <c r="H639" s="85"/>
+      <c r="I639" s="85" t="str">
+        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[openBIS]], 'openBIS - parameters'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
+        <v>Exists</v>
+      </c>
+      <c r="J639" s="86" t="str">
+        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[Ontology]], 'Ontology - definition'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
+        <v>Exists</v>
+      </c>
+      <c r="K639" s="87" t="str">
         <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISBLANK(VLOOKUP(Table1[[#This Row],[Ontology]],'Ontology - definition'!A:B,2,FALSE)),"Doesn't Exist","Exists"),"")</f>
         <v>Exists</v>
       </c>
     </row>
     <row r="640" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A640" s="93" t="s">
+      <c r="A640" s="88" t="s">
         <v>434</v>
       </c>
-      <c r="B640" s="90" t="s">
+      <c r="B640" s="85" t="s">
         <v>990</v>
       </c>
-      <c r="C640" s="90" t="s">
+      <c r="C640" s="85" t="s">
         <v>101</v>
       </c>
-      <c r="D640" s="90" t="s">
+      <c r="D640" s="85" t="s">
         <v>224</v>
       </c>
-      <c r="E640" s="90" t="s">
+      <c r="E640" s="85" t="s">
         <v>903</v>
       </c>
-      <c r="F640" s="90" t="s">
+      <c r="F640" s="85" t="s">
         <v>904</v>
       </c>
-      <c r="G640" s="93" t="s">
+      <c r="G640" s="88" t="s">
         <v>966</v>
       </c>
-      <c r="H640" s="90"/>
-      <c r="I640" s="90" t="str">
-        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[openBIS]], 'openBIS - parameters'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
-        <v>Exists</v>
-      </c>
-      <c r="J640" s="91" t="str">
-        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[Ontology]], 'Ontology - definition'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
-        <v>Exists</v>
-      </c>
-      <c r="K640" s="92" t="str">
+      <c r="H640" s="85"/>
+      <c r="I640" s="85" t="str">
+        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[openBIS]], 'openBIS - parameters'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
+        <v>Exists</v>
+      </c>
+      <c r="J640" s="86" t="str">
+        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[Ontology]], 'Ontology - definition'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
+        <v>Exists</v>
+      </c>
+      <c r="K640" s="87" t="str">
         <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISBLANK(VLOOKUP(Table1[[#This Row],[Ontology]],'Ontology - definition'!A:B,2,FALSE)),"Doesn't Exist","Exists"),"")</f>
         <v>Exists</v>
       </c>
@@ -29283,98 +29232,98 @@
       </c>
     </row>
     <row r="644" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A644" s="93" t="s">
+      <c r="A644" s="88" t="s">
         <v>225</v>
       </c>
-      <c r="B644" s="90" t="s">
+      <c r="B644" s="85" t="s">
         <v>990</v>
       </c>
-      <c r="C644" s="90" t="s">
+      <c r="C644" s="85" t="s">
         <v>101</v>
       </c>
-      <c r="D644" s="90" t="s">
+      <c r="D644" s="85" t="s">
         <v>406</v>
       </c>
-      <c r="E644" s="90" t="s">
+      <c r="E644" s="85" t="s">
         <v>893</v>
       </c>
-      <c r="F644" s="90" t="s">
+      <c r="F644" s="85" t="s">
         <v>896</v>
       </c>
-      <c r="G644" s="93" t="s">
+      <c r="G644" s="88" t="s">
         <v>960</v>
       </c>
-      <c r="H644" s="90"/>
-      <c r="I644" s="90" t="str">
-        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[openBIS]], 'openBIS - parameters'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
-        <v>Exists</v>
-      </c>
-      <c r="J644" s="91" t="str">
-        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[Ontology]], 'Ontology - definition'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
-        <v>Exists</v>
-      </c>
-      <c r="K644" s="92" t="str">
+      <c r="H644" s="85"/>
+      <c r="I644" s="85" t="str">
+        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[openBIS]], 'openBIS - parameters'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
+        <v>Exists</v>
+      </c>
+      <c r="J644" s="86" t="str">
+        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[Ontology]], 'Ontology - definition'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
+        <v>Exists</v>
+      </c>
+      <c r="K644" s="87" t="str">
         <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISBLANK(VLOOKUP(Table1[[#This Row],[Ontology]],'Ontology - definition'!A:B,2,FALSE)),"Doesn't Exist","Exists"),"")</f>
         <v>Exists</v>
       </c>
     </row>
     <row r="645" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A645" s="93" t="s">
+      <c r="A645" s="88" t="s">
         <v>434</v>
       </c>
-      <c r="B645" s="90" t="s">
+      <c r="B645" s="85" t="s">
         <v>990</v>
       </c>
-      <c r="C645" s="90" t="s">
+      <c r="C645" s="85" t="s">
         <v>101</v>
       </c>
-      <c r="D645" s="90" t="s">
+      <c r="D645" s="85" t="s">
         <v>224</v>
       </c>
-      <c r="E645" s="90" t="s">
+      <c r="E645" s="85" t="s">
         <v>903</v>
       </c>
-      <c r="F645" s="90" t="s">
+      <c r="F645" s="85" t="s">
         <v>904</v>
       </c>
-      <c r="G645" s="93" t="s">
+      <c r="G645" s="88" t="s">
         <v>966</v>
       </c>
-      <c r="H645" s="90"/>
-      <c r="I645" s="90" t="str">
-        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[openBIS]], 'openBIS - parameters'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
-        <v>Exists</v>
-      </c>
-      <c r="J645" s="91" t="str">
-        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[Ontology]], 'Ontology - definition'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
-        <v>Exists</v>
-      </c>
-      <c r="K645" s="92" t="str">
+      <c r="H645" s="85"/>
+      <c r="I645" s="85" t="str">
+        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[openBIS]], 'openBIS - parameters'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
+        <v>Exists</v>
+      </c>
+      <c r="J645" s="86" t="str">
+        <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISNUMBER(MATCH(Table1[[#This Row],[Ontology]], 'Ontology - definition'!A:A, 0)), "Exists", "Doesn't Exist"), "")</f>
+        <v>Exists</v>
+      </c>
+      <c r="K645" s="87" t="str">
         <f>IF(Table1[[#This Row],[Ontology]]&lt;&gt;"", IF(ISBLANK(VLOOKUP(Table1[[#This Row],[Ontology]],'Ontology - definition'!A:B,2,FALSE)),"Doesn't Exist","Exists"),"")</f>
         <v>Exists</v>
       </c>
     </row>
     <row r="646" spans="1:11" s="60" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A646" s="62" t="s">
-        <v>1980</v>
-      </c>
-      <c r="B646" s="94" t="s">
+        <v>1967</v>
+      </c>
+      <c r="B646" s="89" t="s">
         <v>1552</v>
       </c>
-      <c r="C646" s="94" t="s">
+      <c r="C646" s="89" t="s">
         <v>100</v>
       </c>
       <c r="D646" s="62" t="s">
-        <v>1980</v>
+        <v>1967</v>
       </c>
       <c r="E646" s="62" t="s">
-        <v>1981</v>
+        <v>1968</v>
       </c>
       <c r="F646" s="62" t="s">
-        <v>1981</v>
+        <v>1968</v>
       </c>
       <c r="G646" s="62" t="s">
-        <v>1982</v>
+        <v>1969</v>
       </c>
       <c r="H646" s="62"/>
       <c r="I646" s="58" t="str">
@@ -33773,551 +33722,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D52"/>
-  <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="29.7109375" customWidth="1"/>
-    <col min="2" max="2" width="107.7109375" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="86" t="s">
-        <v>1045</v>
-      </c>
-      <c r="B1" s="87" t="s">
-        <v>657</v>
-      </c>
-      <c r="C1" s="88" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="44" t="s">
-        <v>1760</v>
-      </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="89" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="48" t="s">
-        <v>506</v>
-      </c>
-      <c r="B3" s="64" t="s">
-        <v>1964</v>
-      </c>
-      <c r="C3" s="26" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="48" t="s">
-        <v>530</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>1965</v>
-      </c>
-      <c r="C4" s="26" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="48" t="s">
-        <v>507</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>1976</v>
-      </c>
-      <c r="C5" s="26" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="48" t="s">
-        <v>1648</v>
-      </c>
-      <c r="B6" s="45"/>
-      <c r="C6" s="26" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="48" t="s">
-        <v>146</v>
-      </c>
-      <c r="B7" s="47" t="s">
-        <v>584</v>
-      </c>
-      <c r="C7" s="26" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="48" t="s">
-        <v>188</v>
-      </c>
-      <c r="B8" s="47"/>
-      <c r="C8" s="26" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="65" t="s">
-        <v>665</v>
-      </c>
-      <c r="B9" s="30"/>
-      <c r="C9" s="66" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="48" t="s">
-        <v>534</v>
-      </c>
-      <c r="B10" s="64" t="s">
-        <v>1966</v>
-      </c>
-      <c r="C10" s="26" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="48" t="s">
-        <v>512</v>
-      </c>
-      <c r="B11" s="64" t="s">
-        <v>536</v>
-      </c>
-      <c r="C11" s="26" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="48" t="s">
-        <v>511</v>
-      </c>
-      <c r="B12" s="64" t="s">
-        <v>1967</v>
-      </c>
-      <c r="C12" s="26" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="48" t="s">
-        <v>192</v>
-      </c>
-      <c r="B13" s="64" t="s">
-        <v>1968</v>
-      </c>
-      <c r="C13" s="26" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="48" t="s">
-        <v>193</v>
-      </c>
-      <c r="B14" s="64" t="s">
-        <v>536</v>
-      </c>
-      <c r="C14" s="26" t="s">
-        <v>1046</v>
-      </c>
-      <c r="D14" t="s">
-        <v>1969</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="65" t="s">
-        <v>670</v>
-      </c>
-      <c r="B15" s="30"/>
-      <c r="C15" s="66" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="44" t="s">
-        <v>491</v>
-      </c>
-      <c r="B16" s="45"/>
-      <c r="C16" s="26" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="73" t="s">
-        <v>679</v>
-      </c>
-      <c r="B17" s="30"/>
-      <c r="C17" s="66" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="44" t="s">
-        <v>541</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>1970</v>
-      </c>
-      <c r="C18" s="26" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="67" t="s">
-        <v>686</v>
-      </c>
-      <c r="B19" s="30"/>
-      <c r="C19" s="66" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="44" t="s">
-        <v>689</v>
-      </c>
-      <c r="B20" s="45"/>
-      <c r="C20" s="26" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="73" t="s">
-        <v>690</v>
-      </c>
-      <c r="B21" s="30"/>
-      <c r="C21" s="66" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="44" t="s">
-        <v>691</v>
-      </c>
-      <c r="B22" s="47"/>
-      <c r="C22" s="26" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="44" t="s">
-        <v>515</v>
-      </c>
-      <c r="B23" s="47"/>
-      <c r="C23" s="26" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="44" t="s">
-        <v>513</v>
-      </c>
-      <c r="B24" s="45"/>
-      <c r="C24" s="26" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="44" t="s">
-        <v>514</v>
-      </c>
-      <c r="B25" s="45"/>
-      <c r="C25" s="26" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="44" t="s">
-        <v>162</v>
-      </c>
-      <c r="B26" s="64" t="s">
-        <v>1971</v>
-      </c>
-      <c r="C26" s="26" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="73" t="s">
-        <v>700</v>
-      </c>
-      <c r="B27" s="85"/>
-      <c r="C27" s="66" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="44" t="s">
-        <v>516</v>
-      </c>
-      <c r="B28" s="45"/>
-      <c r="C28" s="26" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="44" t="s">
-        <v>2</v>
-      </c>
-      <c r="B29" s="45"/>
-      <c r="C29" s="26" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="44" t="s">
-        <v>550</v>
-      </c>
-      <c r="B30" s="45"/>
-      <c r="C30" s="26" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="44" t="s">
-        <v>552</v>
-      </c>
-      <c r="B31" s="45"/>
-      <c r="C31" s="26" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="44" t="s">
-        <v>889</v>
-      </c>
-      <c r="B32" s="22"/>
-      <c r="C32" s="26" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="44" t="s">
-        <v>905</v>
-      </c>
-      <c r="B33" s="47"/>
-      <c r="C33" s="26" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="46" t="s">
-        <v>929</v>
-      </c>
-      <c r="B34" s="22"/>
-      <c r="C34" s="26" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="46" t="s">
-        <v>940</v>
-      </c>
-      <c r="B35" s="22"/>
-      <c r="C35" s="26" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="49" t="s">
-        <v>1436</v>
-      </c>
-      <c r="B36" s="23"/>
-      <c r="C36" s="27" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="46" t="s">
-        <v>556</v>
-      </c>
-      <c r="B37" s="22"/>
-      <c r="C37" s="26" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="44" t="s">
-        <v>509</v>
-      </c>
-      <c r="B38" s="47"/>
-      <c r="C38" s="26" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="73" t="s">
-        <v>942</v>
-      </c>
-      <c r="B39" s="30"/>
-      <c r="C39" s="66" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="44" t="s">
-        <v>1483</v>
-      </c>
-      <c r="B40" s="22"/>
-      <c r="C40" s="26" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="44" t="s">
-        <v>1489</v>
-      </c>
-      <c r="B41" s="22"/>
-      <c r="C41" s="26" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="44" t="s">
-        <v>1519</v>
-      </c>
-      <c r="B42" s="22"/>
-      <c r="C42" s="26" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="44" t="s">
-        <v>1658</v>
-      </c>
-      <c r="B43" s="22"/>
-      <c r="C43" s="26" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="44" t="s">
-        <v>1504</v>
-      </c>
-      <c r="B44" s="64" t="s">
-        <v>1975</v>
-      </c>
-      <c r="C44" s="26" t="s">
-        <v>1046</v>
-      </c>
-      <c r="D44" t="s">
-        <v>1974</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="44" t="s">
-        <v>1506</v>
-      </c>
-      <c r="B45" s="22"/>
-      <c r="C45" s="26" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="67" t="s">
-        <v>1655</v>
-      </c>
-      <c r="B46" s="30"/>
-      <c r="C46" s="66" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="44" t="s">
-        <v>1708</v>
-      </c>
-      <c r="B47" s="64" t="s">
-        <v>1973</v>
-      </c>
-      <c r="C47" s="26" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="44" t="s">
-        <v>1698</v>
-      </c>
-      <c r="B48" s="64" t="s">
-        <v>1972</v>
-      </c>
-      <c r="C48" s="26" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="44" t="s">
-        <v>1705</v>
-      </c>
-      <c r="B49" s="22"/>
-      <c r="C49" s="26" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="44" t="s">
-        <v>1748</v>
-      </c>
-      <c r="B50" s="22"/>
-      <c r="C50" s="26" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="44" t="s">
-        <v>1747</v>
-      </c>
-      <c r="B51" s="22"/>
-      <c r="C51" s="26" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="44" t="s">
-        <v>1749</v>
-      </c>
-      <c r="B52" s="22"/>
-      <c r="C52" s="26" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1"/>
-    <hyperlink ref="B10" r:id="rId2"/>
-    <hyperlink ref="B12" r:id="rId3"/>
-    <hyperlink ref="B18" r:id="rId4"/>
-    <hyperlink ref="B4" r:id="rId5"/>
-    <hyperlink ref="B5" r:id="rId6"/>
-    <hyperlink ref="B3" r:id="rId7"/>
-    <hyperlink ref="B13" r:id="rId8"/>
-    <hyperlink ref="B14" r:id="rId9"/>
-    <hyperlink ref="B11" r:id="rId10"/>
-    <hyperlink ref="B26" r:id="rId11"/>
-    <hyperlink ref="B48" r:id="rId12"/>
-    <hyperlink ref="B47" r:id="rId13"/>
-    <hyperlink ref="B44" r:id="rId14"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:K256"/>
   <sheetViews>
-    <sheetView topLeftCell="A243" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A243" workbookViewId="0">
       <selection activeCell="F256" sqref="F256"/>
     </sheetView>
   </sheetViews>
@@ -39294,7 +38702,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:E33"/>
@@ -39549,7 +38957,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D48"/>
   <sheetViews>
@@ -40246,7 +39654,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>

</xml_diff>